<commit_message>
regjistri per kadaster i kateve
</commit_message>
<xml_diff>
--- a/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-953-5-TalJer-Faruki-leg.xlsx
+++ b/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-953-5-TalJer-Faruki-leg.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Talinoc-i-Jerlive\INXHINIERIKE\513-4-Agimi-legalizim\ob1\4-Te-dhenat-per-kataster\regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Talinoc-i-Jerlive\INXHINIERIKE\953-5-TalJer-Faruki-leg\4-Te-dhenat-per-kataster\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A7E8EE-D330-4B2D-9A7A-0CF1F0CAB70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DD75D0-7AA6-4115-9656-0314F8DF4011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="195" windowWidth="27795" windowHeight="16005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$A$1:$P$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$A$1:$P$22</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
   <si>
     <t>Nr</t>
   </si>
@@ -135,23 +135,16 @@
     <t>Talinoc I Jerlive</t>
   </si>
   <si>
-    <t>Rr."Hamit Troni"</t>
-  </si>
-  <si>
     <t>BREGU</t>
   </si>
   <si>
-    <t>Bodrumi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O-72217046-00513-4-___-0
-</t>
-  </si>
-  <si>
-    <t>B+P+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agim (Hajdar) Spahiu
+    <t>O-72217046-00953-5-___-0</t>
+  </si>
+  <si>
+    <t>Rr. "Qazim Mani"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faruk (Hasan) Lipovica
 </t>
   </si>
 </sst>
@@ -557,13 +550,55 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -589,48 +624,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1021,10 +1014,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P669"/>
+  <dimension ref="A1:P668"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:P8"/>
+      <selection activeCell="P11" sqref="P11:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,170 +1040,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
     </row>
     <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="30"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1246,11 +1239,11 @@
       <c r="K10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
       <c r="O10" s="8" t="s">
         <v>9</v>
       </c>
@@ -1259,173 +1252,152 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
+      <c r="A11" s="21">
         <v>1</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="11">
+        <v>65.67</v>
+      </c>
+      <c r="H11" s="23">
+        <v>65.67</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="11">
-        <v>87.6</v>
-      </c>
-      <c r="H11" s="17">
-        <v>85.68</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="17">
-        <v>1011598036</v>
-      </c>
-      <c r="P11" s="35" t="s">
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="23">
+        <v>1172322731</v>
+      </c>
+      <c r="P11" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="11">
-        <v>85.68</v>
-      </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="36"/>
-    </row>
-    <row r="13" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="15" t="s">
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="16">
-        <v>95.1</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="36"/>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="10" t="s">
+      <c r="G12" s="16">
+        <v>65.67</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="32"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="10">
-        <f>SUM(G11:G13)</f>
-        <v>268.38</v>
-      </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="37"/>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G13" s="10">
+        <f>SUM(G11:G12)</f>
+        <v>131.34</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="28"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+    <row r="20" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="24" t="s">
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24" t="s">
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="26"/>
-    </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="27"/>
-    </row>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="40"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="41"/>
+    </row>
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1454,504 +1426,521 @@
     <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="19"/>
+    </row>
     <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L54" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="M54" s="20"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P54" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="21">
+        <v>1</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="11">
+        <v>99.57</v>
+      </c>
+      <c r="H55" s="23">
+        <v>78.28</v>
+      </c>
+      <c r="I55" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J55" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K55" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="25"/>
+      <c r="O55" s="23"/>
+      <c r="P55" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="29"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" s="16">
+        <v>82.83</v>
+      </c>
+      <c r="H56" s="30"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="30"/>
+      <c r="K56" s="30"/>
+      <c r="L56" s="31"/>
+      <c r="M56" s="31"/>
+      <c r="N56" s="31"/>
+      <c r="O56" s="30"/>
+      <c r="P56" s="32"/>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="22"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" s="10">
+        <f>SUM(G55:G56)</f>
+        <v>182.39999999999998</v>
+      </c>
+      <c r="H57" s="24"/>
+      <c r="I57" s="24"/>
+      <c r="J57" s="24"/>
+      <c r="K57" s="24"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="26"/>
+      <c r="N57" s="26"/>
+      <c r="O57" s="24"/>
+      <c r="P57" s="28"/>
+    </row>
+    <row r="58" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+    </row>
+    <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="29"/>
-      <c r="O54" s="29"/>
-      <c r="P54" s="30"/>
-    </row>
-    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="19"/>
+    </row>
+    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D60" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F60" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="G60" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H60" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="I60" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="J60" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K55" s="8" t="s">
+      <c r="K60" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L55" s="31" t="s">
+      <c r="L60" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="M55" s="31"/>
-      <c r="N55" s="31"/>
-      <c r="O55" s="8" t="s">
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="P55" s="7" t="s">
+      <c r="P60" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="38">
+    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="21">
         <v>1</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B61" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C61" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" s="17" t="s">
+      <c r="D61" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F61" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G56" s="11">
-        <v>99.57</v>
-      </c>
-      <c r="H56" s="17">
-        <v>78.28</v>
-      </c>
-      <c r="I56" s="17" t="s">
+      <c r="G61" s="11">
+        <v>172.23</v>
+      </c>
+      <c r="H61" s="23">
+        <v>158.25</v>
+      </c>
+      <c r="I61" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J56" s="17" t="s">
+      <c r="J61" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K56" s="17" t="s">
+      <c r="K61" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="L56" s="32"/>
-      <c r="M56" s="32"/>
-      <c r="N56" s="32"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="35" t="s">
+      <c r="L61" s="25"/>
+      <c r="M61" s="25"/>
+      <c r="N61" s="25"/>
+      <c r="O61" s="23"/>
+      <c r="P61" s="27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="39"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="15" t="s">
+    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="29"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G57" s="16">
-        <v>82.83</v>
-      </c>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="33"/>
-      <c r="O57" s="18"/>
-      <c r="P57" s="36"/>
-    </row>
-    <row r="58" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="40"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="10" t="s">
+      <c r="G62" s="16">
+        <v>102.44</v>
+      </c>
+      <c r="H62" s="30"/>
+      <c r="I62" s="30"/>
+      <c r="J62" s="30"/>
+      <c r="K62" s="30"/>
+      <c r="L62" s="31"/>
+      <c r="M62" s="31"/>
+      <c r="N62" s="31"/>
+      <c r="O62" s="30"/>
+      <c r="P62" s="32"/>
+    </row>
+    <row r="63" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="22"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G58" s="10">
-        <f>SUM(G56:G57)</f>
-        <v>182.39999999999998</v>
-      </c>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="34"/>
-      <c r="M58" s="34"/>
-      <c r="N58" s="34"/>
-      <c r="O58" s="19"/>
-      <c r="P58" s="37"/>
-    </row>
-    <row r="59" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-      <c r="K59" s="12"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
-      <c r="O59" s="12"/>
-      <c r="P59" s="12"/>
-    </row>
-    <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="G63" s="10">
+        <f>SUM(G61:G62)</f>
+        <v>274.66999999999996</v>
+      </c>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
+      <c r="K63" s="24"/>
+      <c r="L63" s="26"/>
+      <c r="M63" s="26"/>
+      <c r="N63" s="26"/>
+      <c r="O63" s="24"/>
+      <c r="P63" s="28"/>
+    </row>
+    <row r="64" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12"/>
+    </row>
+    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="29"/>
-      <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="29"/>
-      <c r="N60" s="29"/>
-      <c r="O60" s="29"/>
-      <c r="P60" s="30"/>
-    </row>
-    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="19"/>
+    </row>
+    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B66" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D66" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F61" s="8" t="s">
+      <c r="F66" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="8" t="s">
+      <c r="G66" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H61" s="8" t="s">
+      <c r="H66" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I61" s="8" t="s">
+      <c r="I66" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J61" s="8" t="s">
+      <c r="J66" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K61" s="8" t="s">
+      <c r="K66" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L61" s="31" t="s">
+      <c r="L66" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="M61" s="31"/>
-      <c r="N61" s="31"/>
-      <c r="O61" s="8" t="s">
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="P61" s="7" t="s">
+      <c r="P66" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="38">
+    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="21">
         <v>1</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B67" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="C67" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E62" s="17" t="s">
+      <c r="D67" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E67" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F67" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G62" s="11">
-        <v>172.23</v>
-      </c>
-      <c r="H62" s="17">
-        <v>158.25</v>
-      </c>
-      <c r="I62" s="17" t="s">
+      <c r="G67" s="11">
+        <v>160.27000000000001</v>
+      </c>
+      <c r="H67" s="23">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="I67" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J62" s="17" t="s">
+      <c r="J67" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K62" s="17" t="s">
+      <c r="K67" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="L62" s="32"/>
-      <c r="M62" s="32"/>
-      <c r="N62" s="32"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="35" t="s">
+      <c r="L67" s="25"/>
+      <c r="M67" s="25"/>
+      <c r="N67" s="25"/>
+      <c r="O67" s="23"/>
+      <c r="P67" s="27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="39"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="15" t="s">
+    <row r="68" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="29"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G63" s="16">
-        <v>102.44</v>
-      </c>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
-      <c r="L63" s="33"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="33"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="36"/>
-    </row>
-    <row r="64" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="40"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="10" t="s">
+      <c r="G68" s="16">
+        <v>163.03</v>
+      </c>
+      <c r="H68" s="30"/>
+      <c r="I68" s="30"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="30"/>
+      <c r="L68" s="31"/>
+      <c r="M68" s="31"/>
+      <c r="N68" s="31"/>
+      <c r="O68" s="30"/>
+      <c r="P68" s="32"/>
+    </row>
+    <row r="69" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="22"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G64" s="10">
-        <f>SUM(G62:G63)</f>
-        <v>274.66999999999996</v>
-      </c>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
-      <c r="L64" s="34"/>
-      <c r="M64" s="34"/>
-      <c r="N64" s="34"/>
-      <c r="O64" s="19"/>
-      <c r="P64" s="37"/>
-    </row>
-    <row r="65" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-      <c r="O65" s="12"/>
-      <c r="P65" s="12"/>
-    </row>
-    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" s="29"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="29"/>
-      <c r="I66" s="29"/>
-      <c r="J66" s="29"/>
-      <c r="K66" s="29"/>
-      <c r="L66" s="29"/>
-      <c r="M66" s="29"/>
-      <c r="N66" s="29"/>
-      <c r="O66" s="29"/>
-      <c r="P66" s="30"/>
-    </row>
-    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I67" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J67" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K67" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L67" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="M67" s="31"/>
-      <c r="N67" s="31"/>
-      <c r="O67" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="P67" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="38">
-        <v>1</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="11">
-        <v>160.27000000000001</v>
-      </c>
-      <c r="H68" s="17">
-        <v>140.30000000000001</v>
-      </c>
-      <c r="I68" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J68" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="K68" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="32"/>
-      <c r="M68" s="32"/>
-      <c r="N68" s="32"/>
-      <c r="O68" s="17"/>
-      <c r="P68" s="35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="39"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G69" s="16">
-        <v>163.03</v>
-      </c>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-      <c r="L69" s="33"/>
-      <c r="M69" s="33"/>
-      <c r="N69" s="33"/>
-      <c r="O69" s="18"/>
-      <c r="P69" s="36"/>
-    </row>
-    <row r="70" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="40"/>
-      <c r="B70" s="19"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G70" s="10">
-        <f>SUM(G68:G69)</f>
+      <c r="G69" s="10">
+        <f>SUM(G67:G68)</f>
         <v>323.3</v>
       </c>
-      <c r="H70" s="19"/>
-      <c r="I70" s="19"/>
-      <c r="J70" s="19"/>
-      <c r="K70" s="19"/>
-      <c r="L70" s="34"/>
-      <c r="M70" s="34"/>
-      <c r="N70" s="34"/>
-      <c r="O70" s="19"/>
-      <c r="P70" s="37"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H69" s="24"/>
+      <c r="I69" s="24"/>
+      <c r="J69" s="24"/>
+      <c r="K69" s="24"/>
+      <c r="L69" s="26"/>
+      <c r="M69" s="26"/>
+      <c r="N69" s="26"/>
+      <c r="O69" s="24"/>
+      <c r="P69" s="28"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="14"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="12"/>
+      <c r="P70" s="12"/>
+    </row>
+    <row r="71" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
@@ -1969,163 +1958,168 @@
       <c r="O71" s="12"/>
       <c r="P71" s="12"/>
     </row>
-    <row r="72" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="12"/>
-      <c r="K72" s="12"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
-      <c r="O72" s="12"/>
-      <c r="P72" s="12"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B73" s="29"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
-      <c r="G73" s="29"/>
-      <c r="H73" s="29"/>
-      <c r="I73" s="29"/>
-      <c r="J73" s="29"/>
-      <c r="K73" s="29"/>
-      <c r="L73" s="29"/>
-      <c r="M73" s="29"/>
-      <c r="N73" s="29"/>
-      <c r="O73" s="29"/>
-      <c r="P73" s="30"/>
-    </row>
-    <row r="74" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="18"/>
+      <c r="M72" s="18"/>
+      <c r="N72" s="18"/>
+      <c r="O72" s="18"/>
+      <c r="P72" s="19"/>
+    </row>
+    <row r="73" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B73" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C73" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D73" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E73" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F73" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G74" s="8" t="s">
+      <c r="G73" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H74" s="8" t="s">
+      <c r="H73" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I74" s="8" t="s">
+      <c r="I73" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J74" s="8" t="s">
+      <c r="J73" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K74" s="8" t="s">
+      <c r="K73" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L74" s="31" t="s">
+      <c r="L73" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="M74" s="31"/>
-      <c r="N74" s="31"/>
-      <c r="O74" s="8" t="s">
+      <c r="M73" s="20"/>
+      <c r="N73" s="20"/>
+      <c r="O73" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="P74" s="7" t="s">
+      <c r="P73" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75" s="38">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="21">
         <v>1</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B74" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="C74" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D75" s="17" t="s">
+      <c r="D74" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E74" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F74" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G75" s="11">
+      <c r="G74" s="11">
         <v>113.39</v>
       </c>
-      <c r="H75" s="17">
+      <c r="H74" s="23">
         <v>103.6</v>
       </c>
-      <c r="I75" s="17" t="s">
+      <c r="I74" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J75" s="17" t="s">
+      <c r="J74" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K75" s="17" t="s">
+      <c r="K74" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="L75" s="32"/>
-      <c r="M75" s="32"/>
-      <c r="N75" s="32"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="35" t="s">
+      <c r="L74" s="25"/>
+      <c r="M74" s="25"/>
+      <c r="N74" s="25"/>
+      <c r="O74" s="23"/>
+      <c r="P74" s="27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="40"/>
-      <c r="B76" s="19"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="10" t="s">
+    <row r="75" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="22"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G76" s="10">
-        <f>SUM(G75:G75)</f>
+      <c r="G75" s="10">
+        <f>SUM(G74:G74)</f>
         <v>113.39</v>
       </c>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-      <c r="J76" s="19"/>
-      <c r="K76" s="19"/>
-      <c r="L76" s="34"/>
-      <c r="M76" s="34"/>
-      <c r="N76" s="34"/>
-      <c r="O76" s="19"/>
-      <c r="P76" s="37"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="24"/>
+      <c r="L75" s="26"/>
+      <c r="M75" s="26"/>
+      <c r="N75" s="26"/>
+      <c r="O75" s="24"/>
+      <c r="P75" s="28"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="12"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="12"/>
+      <c r="P76" s="12"/>
+    </row>
+    <row r="77" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
+      <c r="F77" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G77" s="13">
+        <f>G75+G69+G63+G57+G13</f>
+        <v>1025.0999999999999</v>
+      </c>
       <c r="H77" s="12"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -2136,28 +2130,8 @@
       <c r="O77" s="12"/>
       <c r="P77" s="12"/>
     </row>
-    <row r="78" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G78" s="13">
-        <f>G76+G70+G64+G58+G14</f>
-        <v>1162.1399999999999</v>
-      </c>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
-      <c r="K78" s="12"/>
-      <c r="L78" s="14"/>
-      <c r="M78" s="14"/>
-      <c r="N78" s="14"/>
-      <c r="O78" s="12"/>
-      <c r="P78" s="12"/>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P78" s="4"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P79" s="4"/>
@@ -2165,8 +2139,8 @@
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P80" s="4"/>
     </row>
-    <row r="81" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P81" s="4"/>
+    <row r="99" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P99" s="4"/>
     </row>
     <row r="100" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P100" s="4"/>
@@ -2174,8 +2148,8 @@
     <row r="101" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P101" s="4"/>
     </row>
-    <row r="102" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P102" s="4"/>
+    <row r="120" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P120" s="4"/>
     </row>
     <row r="121" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P121" s="4"/>
@@ -2183,8 +2157,8 @@
     <row r="122" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P122" s="4"/>
     </row>
-    <row r="123" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P123" s="4"/>
+    <row r="141" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P141" s="4"/>
     </row>
     <row r="142" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P142" s="4"/>
@@ -2192,8 +2166,8 @@
     <row r="143" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P143" s="4"/>
     </row>
-    <row r="144" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P144" s="4"/>
+    <row r="162" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P162" s="4"/>
     </row>
     <row r="163" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P163" s="4"/>
@@ -2201,8 +2175,8 @@
     <row r="164" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P164" s="4"/>
     </row>
-    <row r="165" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P165" s="4"/>
+    <row r="183" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P183" s="4"/>
     </row>
     <row r="184" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P184" s="4"/>
@@ -2210,8 +2184,8 @@
     <row r="185" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P185" s="4"/>
     </row>
-    <row r="186" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P186" s="4"/>
+    <row r="204" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P204" s="4"/>
     </row>
     <row r="205" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P205" s="4"/>
@@ -2219,8 +2193,8 @@
     <row r="206" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P206" s="4"/>
     </row>
-    <row r="207" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P207" s="4"/>
+    <row r="225" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P225" s="4"/>
     </row>
     <row r="226" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P226" s="4"/>
@@ -2228,8 +2202,8 @@
     <row r="227" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P227" s="4"/>
     </row>
-    <row r="228" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P228" s="4"/>
+    <row r="246" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P246" s="4"/>
     </row>
     <row r="247" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P247" s="4"/>
@@ -2237,8 +2211,8 @@
     <row r="248" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P248" s="4"/>
     </row>
-    <row r="249" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P249" s="4"/>
+    <row r="267" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P267" s="4"/>
     </row>
     <row r="268" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P268" s="4"/>
@@ -2246,8 +2220,8 @@
     <row r="269" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P269" s="4"/>
     </row>
-    <row r="270" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P270" s="4"/>
+    <row r="288" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P288" s="4"/>
     </row>
     <row r="289" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P289" s="4"/>
@@ -2255,8 +2229,8 @@
     <row r="290" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P290" s="4"/>
     </row>
-    <row r="291" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P291" s="4"/>
+    <row r="309" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P309" s="4"/>
     </row>
     <row r="310" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P310" s="4"/>
@@ -2264,8 +2238,8 @@
     <row r="311" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P311" s="4"/>
     </row>
-    <row r="312" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P312" s="4"/>
+    <row r="330" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P330" s="4"/>
     </row>
     <row r="331" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P331" s="4"/>
@@ -2273,8 +2247,8 @@
     <row r="332" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P332" s="4"/>
     </row>
-    <row r="333" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P333" s="4"/>
+    <row r="351" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P351" s="4"/>
     </row>
     <row r="352" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P352" s="4"/>
@@ -2282,8 +2256,8 @@
     <row r="353" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P353" s="4"/>
     </row>
-    <row r="354" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P354" s="4"/>
+    <row r="372" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P372" s="4"/>
     </row>
     <row r="373" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P373" s="4"/>
@@ -2291,8 +2265,8 @@
     <row r="374" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P374" s="4"/>
     </row>
-    <row r="375" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P375" s="4"/>
+    <row r="393" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P393" s="4"/>
     </row>
     <row r="394" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P394" s="4"/>
@@ -2300,8 +2274,8 @@
     <row r="395" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P395" s="4"/>
     </row>
-    <row r="396" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P396" s="4"/>
+    <row r="414" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P414" s="4"/>
     </row>
     <row r="415" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P415" s="4"/>
@@ -2309,8 +2283,8 @@
     <row r="416" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P416" s="4"/>
     </row>
-    <row r="417" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P417" s="4"/>
+    <row r="435" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P435" s="4"/>
     </row>
     <row r="436" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P436" s="4"/>
@@ -2318,8 +2292,8 @@
     <row r="437" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P437" s="4"/>
     </row>
-    <row r="438" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P438" s="4"/>
+    <row r="456" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P456" s="4"/>
     </row>
     <row r="457" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P457" s="4"/>
@@ -2327,8 +2301,8 @@
     <row r="458" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P458" s="4"/>
     </row>
-    <row r="459" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P459" s="4"/>
+    <row r="477" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P477" s="4"/>
     </row>
     <row r="478" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P478" s="4"/>
@@ -2336,8 +2310,8 @@
     <row r="479" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P479" s="4"/>
     </row>
-    <row r="480" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P480" s="4"/>
+    <row r="498" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P498" s="4"/>
     </row>
     <row r="499" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P499" s="4"/>
@@ -2345,8 +2319,8 @@
     <row r="500" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P500" s="4"/>
     </row>
-    <row r="501" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P501" s="4"/>
+    <row r="519" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P519" s="4"/>
     </row>
     <row r="520" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P520" s="4"/>
@@ -2354,8 +2328,8 @@
     <row r="521" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P521" s="4"/>
     </row>
-    <row r="522" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P522" s="4"/>
+    <row r="540" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P540" s="4"/>
     </row>
     <row r="541" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P541" s="4"/>
@@ -2363,8 +2337,8 @@
     <row r="542" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P542" s="4"/>
     </row>
-    <row r="543" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P543" s="4"/>
+    <row r="561" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P561" s="4"/>
     </row>
     <row r="562" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P562" s="4"/>
@@ -2372,8 +2346,8 @@
     <row r="563" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P563" s="4"/>
     </row>
-    <row r="564" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P564" s="4"/>
+    <row r="582" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P582" s="4"/>
     </row>
     <row r="583" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P583" s="4"/>
@@ -2381,8 +2355,8 @@
     <row r="584" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P584" s="4"/>
     </row>
-    <row r="585" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P585" s="4"/>
+    <row r="603" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P603" s="4"/>
     </row>
     <row r="604" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P604" s="4"/>
@@ -2390,8 +2364,8 @@
     <row r="605" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P605" s="4"/>
     </row>
-    <row r="606" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P606" s="4"/>
+    <row r="624" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P624" s="4"/>
     </row>
     <row r="625" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P625" s="4"/>
@@ -2399,8 +2373,8 @@
     <row r="626" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P626" s="4"/>
     </row>
-    <row r="627" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P627" s="4"/>
+    <row r="645" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P645" s="4"/>
     </row>
     <row r="646" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P646" s="4"/>
@@ -2408,8 +2382,8 @@
     <row r="647" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P647" s="4"/>
     </row>
-    <row r="648" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P648" s="4"/>
+    <row r="666" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P666" s="4"/>
     </row>
     <row r="667" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P667" s="4"/>
@@ -2417,86 +2391,83 @@
     <row r="668" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P668" s="4"/>
     </row>
-    <row r="669" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P669" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="A73:P73"/>
-    <mergeCell ref="L74:N74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="I75:I76"/>
-    <mergeCell ref="J75:J76"/>
-    <mergeCell ref="K75:K76"/>
-    <mergeCell ref="L75:N76"/>
-    <mergeCell ref="O75:O76"/>
-    <mergeCell ref="P75:P76"/>
-    <mergeCell ref="A66:P66"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="H68:H70"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="J68:J70"/>
-    <mergeCell ref="K68:K70"/>
-    <mergeCell ref="L68:N70"/>
-    <mergeCell ref="O68:O70"/>
-    <mergeCell ref="P68:P70"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="I55:I57"/>
+    <mergeCell ref="J55:J57"/>
+    <mergeCell ref="O55:O57"/>
+    <mergeCell ref="O61:O63"/>
+    <mergeCell ref="P61:P63"/>
+    <mergeCell ref="L60:N60"/>
+    <mergeCell ref="H61:H63"/>
+    <mergeCell ref="I61:I63"/>
+    <mergeCell ref="J61:J63"/>
+    <mergeCell ref="K61:K63"/>
+    <mergeCell ref="L61:N63"/>
+    <mergeCell ref="A59:P59"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="A4:P8"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="A21:D22"/>
+    <mergeCell ref="E21:H22"/>
+    <mergeCell ref="I21:P22"/>
+    <mergeCell ref="A53:P53"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="K55:K57"/>
+    <mergeCell ref="L55:N57"/>
+    <mergeCell ref="P55:P57"/>
+    <mergeCell ref="H55:H57"/>
     <mergeCell ref="A1:P3"/>
     <mergeCell ref="A9:P9"/>
     <mergeCell ref="L10:N10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="J11:J14"/>
-    <mergeCell ref="K11:K14"/>
-    <mergeCell ref="O11:O14"/>
-    <mergeCell ref="P11:P14"/>
-    <mergeCell ref="L11:N14"/>
-    <mergeCell ref="A60:P60"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="A4:P8"/>
-    <mergeCell ref="O62:O64"/>
-    <mergeCell ref="P62:P64"/>
-    <mergeCell ref="L61:N61"/>
-    <mergeCell ref="H62:H64"/>
-    <mergeCell ref="I62:I64"/>
-    <mergeCell ref="J62:J64"/>
-    <mergeCell ref="K62:K64"/>
-    <mergeCell ref="L62:N64"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="A22:D23"/>
-    <mergeCell ref="E22:H23"/>
-    <mergeCell ref="I22:P23"/>
-    <mergeCell ref="A54:P54"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="K56:K58"/>
-    <mergeCell ref="L56:N58"/>
-    <mergeCell ref="P56:P58"/>
-    <mergeCell ref="H56:H58"/>
-    <mergeCell ref="I56:I58"/>
-    <mergeCell ref="J56:J58"/>
-    <mergeCell ref="O56:O58"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="P11:P13"/>
+    <mergeCell ref="L11:N13"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="E61:E63"/>
+    <mergeCell ref="A65:P65"/>
+    <mergeCell ref="L66:N66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="D67:D69"/>
+    <mergeCell ref="E67:E69"/>
+    <mergeCell ref="H67:H69"/>
+    <mergeCell ref="I67:I69"/>
+    <mergeCell ref="J67:J69"/>
+    <mergeCell ref="K67:K69"/>
+    <mergeCell ref="L67:N69"/>
+    <mergeCell ref="O67:O69"/>
+    <mergeCell ref="P67:P69"/>
+    <mergeCell ref="A72:P72"/>
+    <mergeCell ref="L73:N73"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="I74:I75"/>
+    <mergeCell ref="J74:J75"/>
+    <mergeCell ref="K74:K75"/>
+    <mergeCell ref="L74:N75"/>
+    <mergeCell ref="O74:O75"/>
+    <mergeCell ref="P74:P75"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>